<commit_message>
Minor changes to the overview file
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moecklb0\Desktop\Statistical Analysis\IGA_maternalobesity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatmockli/Desktop/IGA_maternalobesity/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3E422C-7400-2B49-873D-755BCD5B514A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview Experiments" sheetId="1" r:id="rId1"/>
@@ -20,17 +21,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Relevant genes'!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="396">
   <si>
     <t>10.1371/journal.pone.0090335</t>
   </si>
@@ -1219,12 +1226,15 @@
   </si>
   <si>
     <t>Ye et al., Front End., 2020; Wu et al. 2018</t>
+  </si>
+  <si>
+    <t>Dongiovanni et al., 2013; Mouralidarane et al, 2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1293,7 +1303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1357,6 +1367,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1637,37 +1650,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="5.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.83203125" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1714,7 +1727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1761,7 +1774,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1808,7 +1821,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -1846,7 +1859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -1884,7 +1897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -1928,7 +1941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>103</v>
       </c>
@@ -1972,7 +1985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2019,16 +2032,16 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H10" s="10"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>154</v>
       </c>
@@ -2075,7 +2088,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>132</v>
       </c>
@@ -2122,7 +2135,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2169,13 +2182,13 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>254</v>
       </c>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2219,7 +2232,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>174</v>
       </c>
@@ -2266,7 +2279,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2313,7 +2326,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>229</v>
       </c>
@@ -2360,13 +2373,13 @@
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>289</v>
       </c>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>159</v>
       </c>
@@ -2410,7 +2423,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -2454,7 +2467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>125</v>
       </c>
@@ -2498,13 +2511,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>261</v>
       </c>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2551,7 +2564,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2598,7 +2611,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2645,7 +2658,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>309</v>
       </c>
@@ -2692,7 +2705,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2736,17 +2749,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>248</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2790,7 +2803,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>212</v>
       </c>
@@ -2837,7 +2850,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>290</v>
       </c>
@@ -2878,10 +2891,10 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
         <v>292</v>
       </c>
@@ -2893,7 +2906,7 @@
       </c>
       <c r="I39" s="18"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -2904,7 +2917,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -2915,7 +2928,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -2926,7 +2939,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>
@@ -2937,7 +2950,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>158</v>
       </c>
@@ -2949,7 +2962,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>306</v>
       </c>
@@ -2963,22 +2976,22 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
     </row>
-    <row r="47" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
         <v>293</v>
       </c>
       <c r="I47" s="18"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -2986,7 +2999,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>206</v>
       </c>
@@ -2994,7 +3007,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>228</v>
       </c>
@@ -3004,8 +3017,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://doi.org/10.1371/journal.pone.0090335"/>
-    <hyperlink ref="E4" r:id="rId2" display="https://doi.org/10.1371/journal.pone.0090335"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://doi.org/10.1371/journal.pone.0090335" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId2" display="https://doi.org/10.1371/journal.pone.0090335" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
@@ -3013,22 +3026,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.85546875" style="25" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.83203125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>341</v>
       </c>
@@ -3054,7 +3067,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>71</v>
       </c>
@@ -3070,7 +3083,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
         <v>245</v>
       </c>
@@ -3090,7 +3103,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>226</v>
       </c>
@@ -3110,7 +3123,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>300</v>
       </c>
@@ -3132,7 +3145,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>324</v>
       </c>
@@ -3152,7 +3165,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>87</v>
       </c>
@@ -3168,7 +3181,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>57</v>
       </c>
@@ -3184,7 +3197,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>92</v>
       </c>
@@ -3200,7 +3213,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>58</v>
       </c>
@@ -3216,7 +3229,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>93</v>
       </c>
@@ -3232,7 +3245,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>362</v>
       </c>
@@ -3250,7 +3263,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>288</v>
       </c>
@@ -3272,7 +3285,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
         <v>84</v>
       </c>
@@ -3288,7 +3301,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
         <v>60</v>
       </c>
@@ -3304,7 +3317,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
         <v>354</v>
       </c>
@@ -3324,7 +3337,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>91</v>
       </c>
@@ -3346,7 +3359,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
         <v>70</v>
       </c>
@@ -3364,7 +3377,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
         <v>349</v>
       </c>
@@ -3382,7 +3395,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>327</v>
       </c>
@@ -3402,7 +3415,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
         <v>204</v>
       </c>
@@ -3422,7 +3435,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
         <v>378</v>
       </c>
@@ -3440,7 +3453,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
         <v>195</v>
       </c>
@@ -3458,7 +3471,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
         <v>321</v>
       </c>
@@ -3478,7 +3491,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
         <v>55</v>
       </c>
@@ -3494,7 +3507,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
         <v>240</v>
       </c>
@@ -3514,7 +3527,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
         <v>56</v>
       </c>
@@ -3530,7 +3543,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
         <v>61</v>
       </c>
@@ -3550,7 +3563,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="26" t="s">
         <v>59</v>
       </c>
@@ -3566,7 +3579,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
         <v>69</v>
       </c>
@@ -3584,7 +3597,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
         <v>301</v>
       </c>
@@ -3604,7 +3617,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
         <v>253</v>
       </c>
@@ -3624,7 +3637,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="26" t="s">
         <v>189</v>
       </c>
@@ -3642,7 +3655,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
         <v>192</v>
       </c>
@@ -3658,7 +3671,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
         <v>185</v>
       </c>
@@ -3676,7 +3689,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="26" t="s">
         <v>221</v>
       </c>
@@ -3696,7 +3709,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="26" t="s">
         <v>356</v>
       </c>
@@ -3716,7 +3729,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
         <v>88</v>
       </c>
@@ -3734,7 +3747,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
         <v>370</v>
       </c>
@@ -3749,10 +3762,10 @@
       </c>
       <c r="G39" s="27"/>
       <c r="H39" s="26" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="26" t="s">
         <v>273</v>
       </c>
@@ -3774,7 +3787,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
         <v>279</v>
       </c>
@@ -3796,7 +3809,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
         <v>382</v>
       </c>
@@ -3812,7 +3825,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="26" t="s">
         <v>371</v>
       </c>
@@ -3827,10 +3840,10 @@
       </c>
       <c r="G43" s="27"/>
       <c r="H43" s="26" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="26" t="s">
         <v>355</v>
       </c>
@@ -3851,8 +3864,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1">
-    <sortState ref="A2:H44">
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H44">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -3862,19 +3875,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="90.140625" customWidth="1"/>
+    <col min="4" max="4" width="90.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>292</v>
       </c>
@@ -3888,7 +3901,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>23</v>
       </c>
@@ -3902,7 +3915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -3913,7 +3926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -3924,7 +3937,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -3935,8 +3948,8 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
         <v>317</v>
       </c>
       <c r="B6" s="24"/>
@@ -3947,7 +3960,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>306</v>
       </c>
@@ -3969,20 +3982,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -3993,7 +4006,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>319</v>
       </c>
@@ -4001,7 +4014,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>392</v>
       </c>
@@ -4012,7 +4025,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>330</v>
       </c>
@@ -4023,7 +4036,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>333</v>
       </c>
@@ -4031,7 +4044,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>334</v>
       </c>
@@ -4039,7 +4052,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>336</v>
       </c>
@@ -4047,7 +4060,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>338</v>
       </c>
@@ -4055,7 +4068,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>342</v>
       </c>
@@ -4063,7 +4076,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>343</v>
       </c>

</xml_diff>

<commit_message>
Save of overview file without conscious changes
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatmockli/Desktop/IGA_maternalobesity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moecklb0\Desktop\Statistical Analysis\IGA_maternalobesity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3E422C-7400-2B49-873D-755BCD5B514A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Overview Experiments" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Relevant genes'!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -651,9 +650,6 @@
     <t>Rev-ErbA-Alpha</t>
   </si>
   <si>
-    <t>Transcriptional repressor, circadian Rhytm, metabolic pathways</t>
-  </si>
-  <si>
     <t>Nr1d1</t>
   </si>
   <si>
@@ -1229,12 +1225,15 @@
   </si>
   <si>
     <t>Dongiovanni et al., 2013; Mouralidarane et al, 2013</t>
+  </si>
+  <si>
+    <t>Transcriptional repressor, circadian Rhytm, various metabolic pathways</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1650,37 +1649,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:G45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="5.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.83203125" customWidth="1"/>
-    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1727,7 +1726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1774,7 +1773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1821,7 +1820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -1897,7 +1896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -1941,7 +1940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>103</v>
       </c>
@@ -1985,7 +1984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2032,16 +2031,16 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H10" s="10"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>154</v>
       </c>
@@ -2055,7 +2054,7 @@
         <v>150</v>
       </c>
       <c r="E12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F12">
         <v>2014</v>
@@ -2088,7 +2087,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>132</v>
       </c>
@@ -2135,18 +2134,18 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
         <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E14" t="s">
         <v>35</v>
@@ -2164,7 +2163,7 @@
         <v>124</v>
       </c>
       <c r="J14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K14" t="s">
         <v>11</v>
@@ -2179,16 +2178,16 @@
         <v>27</v>
       </c>
       <c r="O14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2199,7 +2198,7 @@
         <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E17" t="s">
         <v>38</v>
@@ -2211,7 +2210,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>14</v>
@@ -2223,16 +2222,16 @@
         <v>33</v>
       </c>
       <c r="M17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N17" t="s">
         <v>27</v>
       </c>
       <c r="O17" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>174</v>
       </c>
@@ -2279,7 +2278,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -2317,36 +2316,36 @@
         <v>32</v>
       </c>
       <c r="M19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N19" t="s">
         <v>7</v>
       </c>
       <c r="O19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" t="s">
         <v>229</v>
-      </c>
-      <c r="B20" t="s">
-        <v>230</v>
       </c>
       <c r="C20" t="s">
         <v>100</v>
       </c>
       <c r="D20" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" t="s">
         <v>231</v>
-      </c>
-      <c r="E20" t="s">
-        <v>232</v>
       </c>
       <c r="F20">
         <v>2012</v>
       </c>
       <c r="G20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H20" s="8">
         <v>2</v>
@@ -2355,36 +2354,36 @@
         <v>13</v>
       </c>
       <c r="J20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L20" t="s">
         <v>32</v>
       </c>
       <c r="M20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N20" t="s">
         <v>27</v>
       </c>
       <c r="O20" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>159</v>
       </c>
       <c r="B23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C23" t="s">
         <v>100</v>
@@ -2423,7 +2422,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E24" t="s">
         <v>98</v>
@@ -2443,10 +2442,10 @@
         <v>2015</v>
       </c>
       <c r="G24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>13</v>
@@ -2467,7 +2466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>125</v>
       </c>
@@ -2511,42 +2510,42 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C28" t="s">
         <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F28">
         <v>2013</v>
       </c>
       <c r="G28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K28" t="s">
         <v>11</v>
@@ -2555,7 +2554,7 @@
         <v>32</v>
       </c>
       <c r="M28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N28" t="s">
         <v>27</v>
@@ -2564,7 +2563,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2575,7 +2574,7 @@
         <v>146</v>
       </c>
       <c r="D29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E29" t="s">
         <v>143</v>
@@ -2602,16 +2601,16 @@
         <v>33</v>
       </c>
       <c r="M29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N29" t="s">
         <v>27</v>
       </c>
       <c r="O29" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2658,21 +2657,21 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>308</v>
+      </c>
+      <c r="B31" t="s">
         <v>309</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>310</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>311</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>312</v>
-      </c>
-      <c r="E31" t="s">
-        <v>313</v>
       </c>
       <c r="F31">
         <v>2017</v>
@@ -2696,16 +2695,16 @@
         <v>32</v>
       </c>
       <c r="M31" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N31" t="s">
         <v>27</v>
       </c>
       <c r="O31" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2716,7 +2715,7 @@
         <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
@@ -2728,7 +2727,7 @@
         <v>15</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>14</v>
@@ -2743,23 +2742,23 @@
         <v>33</v>
       </c>
       <c r="M32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2803,9 +2802,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
@@ -2814,7 +2813,7 @@
         <v>100</v>
       </c>
       <c r="D36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E36" t="s">
         <v>122</v>
@@ -2841,18 +2840,18 @@
         <v>50</v>
       </c>
       <c r="M36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N36" t="s">
         <v>27</v>
       </c>
       <c r="O36" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B37" t="s">
         <v>167</v>
@@ -2891,22 +2890,22 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E39" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="G39" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="G39" s="17" t="s">
-        <v>308</v>
-      </c>
       <c r="I39" s="18"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -2928,7 +2927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -2939,7 +2938,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>148</v>
       </c>
@@ -2950,7 +2949,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>158</v>
       </c>
@@ -2962,9 +2961,9 @@
         <v>948</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E45" s="21">
         <f>SUM(E40:E44)</f>
@@ -2976,22 +2975,22 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
     </row>
-    <row r="47" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I47" s="18"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -2999,17 +2998,17 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D50">
         <v>7.41</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D51">
         <v>5.1820000000000004</v>
@@ -3017,8 +3016,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://doi.org/10.1371/journal.pone.0090335" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E4" r:id="rId2" display="https://doi.org/10.1371/journal.pone.0090335" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://doi.org/10.1371/journal.pone.0090335"/>
+    <hyperlink ref="E4" r:id="rId2" display="https://doi.org/10.1371/journal.pone.0090335"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
@@ -3026,24 +3025,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.83203125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>73</v>
@@ -3052,7 +3051,7 @@
         <v>181</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>54</v>
@@ -3067,7 +3066,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>71</v>
       </c>
@@ -3080,92 +3079,92 @@
       <c r="F2" s="26"/>
       <c r="G2" s="27"/>
       <c r="H2" s="26" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B5" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>297</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>298</v>
       </c>
       <c r="E5" s="26"/>
       <c r="F5" s="26"/>
       <c r="G5" s="29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>87</v>
       </c>
@@ -3178,10 +3177,10 @@
       <c r="F7" s="26"/>
       <c r="G7" s="27"/>
       <c r="H7" s="26" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>57</v>
       </c>
@@ -3194,10 +3193,10 @@
       <c r="F8" s="26"/>
       <c r="G8" s="27"/>
       <c r="H8" s="26" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>92</v>
       </c>
@@ -3210,10 +3209,10 @@
       <c r="F9" s="26"/>
       <c r="G9" s="27"/>
       <c r="H9" s="26" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>58</v>
       </c>
@@ -3226,10 +3225,10 @@
       <c r="F10" s="26"/>
       <c r="G10" s="27"/>
       <c r="H10" s="26" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>93</v>
       </c>
@@ -3242,50 +3241,50 @@
       <c r="F11" s="26"/>
       <c r="G11" s="27"/>
       <c r="H11" s="26" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
       <c r="F12" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="26" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B13" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="D13" s="26" t="s">
         <v>285</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>286</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
       <c r="G13" s="27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>84</v>
       </c>
@@ -3298,10 +3297,10 @@
       <c r="F14" s="26"/>
       <c r="G14" s="27"/>
       <c r="H14" s="26" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>60</v>
       </c>
@@ -3314,30 +3313,30 @@
       <c r="F15" s="26"/>
       <c r="G15" s="27"/>
       <c r="H15" s="26" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G16" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="H16" s="26" t="s">
         <v>359</v>
       </c>
-      <c r="H16" s="26" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>91</v>
       </c>
@@ -3345,10 +3344,10 @@
         <v>90</v>
       </c>
       <c r="C17" s="28" t="s">
+        <v>371</v>
+      </c>
+      <c r="D17" s="28" t="s">
         <v>372</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>373</v>
       </c>
       <c r="E17" s="26"/>
       <c r="F17" s="26" t="s">
@@ -3356,10 +3355,10 @@
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="26" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>70</v>
       </c>
@@ -3374,50 +3373,50 @@
       </c>
       <c r="G18" s="27"/>
       <c r="H18" s="26" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G19" s="27"/>
       <c r="H19" s="26" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G20" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="H20" s="26" t="s">
         <v>328</v>
       </c>
-      <c r="H20" s="26" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>201</v>
@@ -3429,31 +3428,31 @@
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="27" t="s">
-        <v>203</v>
+        <v>395</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>378</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>380</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>379</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
       <c r="F22" s="26"/>
       <c r="G22" s="27"/>
       <c r="H22" s="26" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>195</v>
       </c>
@@ -3471,27 +3470,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>55</v>
       </c>
@@ -3504,30 +3503,30 @@
       <c r="F25" s="26"/>
       <c r="G25" s="27"/>
       <c r="H25" s="26" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B26" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="C26" s="28" t="s">
         <v>238</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>239</v>
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="26"/>
       <c r="F26" s="26"/>
       <c r="G26" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H26" s="26" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>56</v>
       </c>
@@ -3540,10 +3539,10 @@
       <c r="F27" s="26"/>
       <c r="G27" s="27"/>
       <c r="H27" s="26" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>61</v>
       </c>
@@ -3563,7 +3562,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>59</v>
       </c>
@@ -3576,10 +3575,10 @@
       <c r="F29" s="26"/>
       <c r="G29" s="27"/>
       <c r="H29" s="26" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>69</v>
       </c>
@@ -3594,50 +3593,50 @@
       </c>
       <c r="G30" s="27"/>
       <c r="H30" s="26" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="B31" s="28" t="s">
         <v>301</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>302</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27" t="s">
+        <v>303</v>
+      </c>
+      <c r="H31" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="H31" s="26" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32" s="26"/>
       <c r="G32" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>189</v>
       </c>
@@ -3655,7 +3654,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>192</v>
       </c>
@@ -3671,7 +3670,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>185</v>
       </c>
@@ -3689,47 +3688,47 @@
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B36" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="C36" s="28" t="s">
         <v>219</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>220</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="26"/>
       <c r="F36" s="26"/>
       <c r="G36" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H36" s="26" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="26"/>
       <c r="F37" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H37" s="26" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>88</v>
       </c>
@@ -3744,77 +3743,77 @@
       <c r="F38" s="26"/>
       <c r="G38" s="27"/>
       <c r="H38" s="26" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" s="26"/>
       <c r="F39" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G39" s="27"/>
       <c r="H39" s="26" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>273</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>274</v>
       </c>
       <c r="C40" s="28"/>
       <c r="D40" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="E40" s="28" t="s">
         <v>275</v>
-      </c>
-      <c r="E40" s="28" t="s">
-        <v>276</v>
       </c>
       <c r="F40" s="26"/>
       <c r="G40" s="29" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H40" s="28" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="B41" s="28" t="s">
         <v>279</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>280</v>
       </c>
       <c r="C41" s="28"/>
       <c r="D41" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="E41" s="28" t="s">
         <v>281</v>
-      </c>
-      <c r="E41" s="28" t="s">
-        <v>282</v>
       </c>
       <c r="F41" s="26"/>
       <c r="G41" s="29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H41" s="28" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="B42" s="26" t="s">
         <v>382</v>
-      </c>
-      <c r="B42" s="26" t="s">
-        <v>383</v>
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
@@ -3822,50 +3821,50 @@
       <c r="F42" s="26"/>
       <c r="G42" s="27"/>
       <c r="H42" s="26" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
       <c r="F43" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G43" s="27"/>
       <c r="H43" s="26" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H44" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H44">
+  <autoFilter ref="A1:H1">
+    <sortState ref="A2:H44">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -3875,33 +3874,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="90.1640625" customWidth="1"/>
+    <col min="4" max="4" width="90.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>23</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -3926,7 +3925,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -3937,7 +3936,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -3948,9 +3947,9 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B6" s="24"/>
       <c r="E6" s="13">
@@ -3960,9 +3959,9 @@
         <v>948</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -3982,109 +3981,109 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>319</v>
-      </c>
       <c r="C2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>333</v>
+      </c>
+      <c r="C6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>392</v>
-      </c>
-      <c r="B3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C4" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>333</v>
-      </c>
-      <c r="C5" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>334</v>
-      </c>
-      <c r="C6" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>336</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
         <v>338</v>
       </c>
-      <c r="C8" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>341</v>
+      </c>
+      <c r="C9" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>342</v>
       </c>
-      <c r="C9" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>343</v>
       </c>
-      <c r="B10" t="s">
-        <v>344</v>
-      </c>
       <c r="C10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed empty fields for the overview file.
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview Experiments" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="relevanPW_NALFD" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Relevant genes'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Relevant genes'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="484">
   <si>
     <t>10.1371/journal.pone.0090335</t>
   </si>
@@ -242,9 +242,6 @@
     <t>(high[All Fields] AND fat[All Fields]) AND offspring[All Fields] AND ("liver"[MeSH Terms] OR liver[All Fields])</t>
   </si>
   <si>
-    <t>Relevance</t>
-  </si>
-  <si>
     <t>Saa1</t>
   </si>
   <si>
@@ -252,9 +249,6 @@
   </si>
   <si>
     <t>Adipoq</t>
-  </si>
-  <si>
-    <t>duplicated</t>
   </si>
   <si>
     <t>human_symbol</t>
@@ -611,9 +605,6 @@
     <t>Sirt1</t>
   </si>
   <si>
-    <t>Longevity, ageing associated cancer</t>
-  </si>
-  <si>
     <t>Borengasser et al., 2014; Bruce et al., 2016</t>
   </si>
   <si>
@@ -638,9 +629,6 @@
     <t>PGC1a</t>
   </si>
   <si>
-    <t>ROS activated, cold exposure</t>
-  </si>
-  <si>
     <t>McCurdy et al., 2009</t>
   </si>
   <si>
@@ -704,18 +692,9 @@
     <t>Socs2</t>
   </si>
   <si>
-    <t>Cytokine signaling, IGF signaling</t>
-  </si>
-  <si>
     <t>CASP6</t>
   </si>
   <si>
-    <t>Caspase</t>
-  </si>
-  <si>
-    <t>Cell apoptosis</t>
-  </si>
-  <si>
     <t>Casp6</t>
   </si>
   <si>
@@ -761,9 +740,6 @@
     <t>Ppard</t>
   </si>
   <si>
-    <t>TF, exercise mimetics,beta-catenin pathway</t>
-  </si>
-  <si>
     <t>APOA4</t>
   </si>
   <si>
@@ -791,9 +767,6 @@
     <t>SERPINA12</t>
   </si>
   <si>
-    <t>Insulin resistance, obeisty</t>
-  </si>
-  <si>
     <t>Serine Protease inhibitor</t>
   </si>
   <si>
@@ -866,9 +839,6 @@
     <t>Tissue Inhibitor of Metalloproteinases 1</t>
   </si>
   <si>
-    <t>Fibrosis related</t>
-  </si>
-  <si>
     <t>Inhibitor of Metalloproteinases</t>
   </si>
   <si>
@@ -887,9 +857,6 @@
     <t>Innate immunity</t>
   </si>
   <si>
-    <t>Response to bacterial lipoproteins</t>
-  </si>
-  <si>
     <t>IGFBP1</t>
   </si>
   <si>
@@ -945,12 +912,6 @@
   </si>
   <si>
     <t>SCD1</t>
-  </si>
-  <si>
-    <t>Stearoyl-CoA Desaturase</t>
-  </si>
-  <si>
-    <t>Lipid synthesis</t>
   </si>
   <si>
     <t>Kamimae-Lanning et al., 2014; Seki et al., 2017; Pruis et al., 2014</t>
@@ -1005,9 +966,6 @@
     <t>Pnpla3</t>
   </si>
   <si>
-    <t>literature search</t>
-  </si>
-  <si>
     <t>COL13A1</t>
   </si>
   <si>
@@ -1023,18 +981,12 @@
     <t>Mttp</t>
   </si>
   <si>
-    <t>Impairs VLDL cholesterol secretion</t>
-  </si>
-  <si>
     <t>Schuster et al., 2018</t>
   </si>
   <si>
     <t>MAPK</t>
   </si>
   <si>
-    <t>MAPK signaling pathway</t>
-  </si>
-  <si>
     <t>PI3K-Akt signaling pathway</t>
   </si>
   <si>
@@ -1065,18 +1017,9 @@
     <t>symbol</t>
   </si>
   <si>
-    <t>Oxidative stress</t>
-  </si>
-  <si>
     <t>TLR</t>
   </si>
   <si>
-    <t xml:space="preserve">Toll-like Receptors </t>
-  </si>
-  <si>
-    <t>Tong et al., 2019</t>
-  </si>
-  <si>
     <t>Seki et al., 2017; Hoang et al., 2019</t>
   </si>
   <si>
@@ -1113,12 +1056,6 @@
     <t>Mitochondrial antioxidant</t>
   </si>
   <si>
-    <t>Mitochondrial lipid metabolism</t>
-  </si>
-  <si>
-    <t>innate immunity, HSC activation</t>
-  </si>
-  <si>
     <t>Eslam et al., 2018</t>
   </si>
   <si>
@@ -1158,9 +1095,6 @@
     <t>ChREBP</t>
   </si>
   <si>
-    <t>LX interacting protein</t>
-  </si>
-  <si>
     <t>Kärst et al., 2015; Hori et al, 2014; Pruis et al., 2014; Parlati et al., 2021</t>
   </si>
   <si>
@@ -1228,6 +1162,336 @@
   </si>
   <si>
     <t>Transcriptional repressor, circadian Rhytm, various metabolic pathways</t>
+  </si>
+  <si>
+    <t>Adiponectin</t>
+  </si>
+  <si>
+    <t>Metabolic and hormonal processes</t>
+  </si>
+  <si>
+    <t>Caspase 6</t>
+  </si>
+  <si>
+    <t>Cell apoptosis and programmed cell death</t>
+  </si>
+  <si>
+    <t>Collagen alpha-1(XIII) chain</t>
+  </si>
+  <si>
+    <t>Protein name</t>
+  </si>
+  <si>
+    <t>Carnitine O-palmitoyltransferase 1</t>
+  </si>
+  <si>
+    <t>Lipid metabolism</t>
+  </si>
+  <si>
+    <t>Catalyzes the transfer of the acyl group of long-chain fatty acid-CoA conjugates onto carnitine</t>
+  </si>
+  <si>
+    <t>Fatty acid synthase</t>
+  </si>
+  <si>
+    <t>catalyzes the de novo biosynthesis of long-chain saturated fatty acids</t>
+  </si>
+  <si>
+    <t>Biological process</t>
+  </si>
+  <si>
+    <t>Fibroblast growth factor 21</t>
+  </si>
+  <si>
+    <t>Important hepatokine with a multitude of metabolic functions</t>
+  </si>
+  <si>
+    <t>Fibroblast growth factor 19</t>
+  </si>
+  <si>
+    <t>Bile acid synthesis</t>
+  </si>
+  <si>
+    <t>Hormone that regulates bile acid synthesis</t>
+  </si>
+  <si>
+    <t>Glucokinase regulatory protein</t>
+  </si>
+  <si>
+    <t>Carbohydrate metabolism</t>
+  </si>
+  <si>
+    <t>Regulates glucokinase by forming an inactive complex with this enzyme</t>
+  </si>
+  <si>
+    <t>Fibroblast growth factor receptor 1</t>
+  </si>
+  <si>
+    <t>Tyrosine-protein kinase that acts as cell-surface receptor for fibroblast growth factors</t>
+  </si>
+  <si>
+    <t>Growth factor receptor binding</t>
+  </si>
+  <si>
+    <t>Growth factor binding</t>
+  </si>
+  <si>
+    <t>Leptin</t>
+  </si>
+  <si>
+    <t>Leptin receptor</t>
+  </si>
+  <si>
+    <t>Key player in the regulation of energy balance and body weight control</t>
+  </si>
+  <si>
+    <t>Receptor for leptin</t>
+  </si>
+  <si>
+    <t>Energy homeostasis</t>
+  </si>
+  <si>
+    <t>Innate immunity, HSC activation</t>
+  </si>
+  <si>
+    <t>Tyrosine-protein kinase Mer</t>
+  </si>
+  <si>
+    <t>Carbohydrate-responsive element-binding protein</t>
+  </si>
+  <si>
+    <t>Transcriptional repressor. Binds to the canonical and non-canonical E box sequences</t>
+  </si>
+  <si>
+    <t>DBH-like monooxygenase protein 1</t>
+  </si>
+  <si>
+    <t>Octopamine biosynthetic process</t>
+  </si>
+  <si>
+    <t>Catalyzes the conversion of dopamine to norepinephrine</t>
+  </si>
+  <si>
+    <t>Catalyzes the reduction of N-oxygenated molecules</t>
+  </si>
+  <si>
+    <t>Mitochondrial amidoxime-reducing component 1</t>
+  </si>
+  <si>
+    <t>Nitrate metabolic process</t>
+  </si>
+  <si>
+    <t>Required for the assembly and secretion of plasma lipoproteins</t>
+  </si>
+  <si>
+    <t>Microsomal triglyceride transfer protein large subunit</t>
+  </si>
+  <si>
+    <t>Nuclear receptor subfamily 1 group D member 1</t>
+  </si>
+  <si>
+    <t>Biological rhytms</t>
+  </si>
+  <si>
+    <t>Bile acid receptor</t>
+  </si>
+  <si>
+    <t>Receptor for bile acids such as chenodeoxycholic acid, lithocholic acid and allocholic acid.</t>
+  </si>
+  <si>
+    <t>Bile acid metabolism</t>
+  </si>
+  <si>
+    <t>Phosphoenolpyruvate carboxykinase</t>
+  </si>
+  <si>
+    <t>Gluconeogenesis</t>
+  </si>
+  <si>
+    <t>1-acylglycerol-3-phosphate O-acyltransferase</t>
+  </si>
+  <si>
+    <t>Peroxisome proliferator-activated receptor alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key regulator of lipid metabolism. Regulates the peroxisomal beta-oxidation pathway of fatty acids. </t>
+  </si>
+  <si>
+    <t>Transcription regulation</t>
+  </si>
+  <si>
+    <t>Transcription factor, exercise mimetics, beta-catenin pathway</t>
+  </si>
+  <si>
+    <t>Peroxisome proliferator-activated receptor delta</t>
+  </si>
+  <si>
+    <t>Peroxisome proliferator-activated receptor gamma</t>
+  </si>
+  <si>
+    <t>Nuclear receptor that binds peroxisome proliferators such as hypolipidemic drugs and fatty acids.</t>
+  </si>
+  <si>
+    <t>Transcriptional coactivator for steroid receptors and nuclear receptors. Greatly increases the transcriptional activity of PPARG.</t>
+  </si>
+  <si>
+    <t>Peroxisome proliferator-activated receptor gamma coactivator 1-alpha</t>
+  </si>
+  <si>
+    <t>Retinoic acid receptor</t>
+  </si>
+  <si>
+    <t>Receptor for retinoic acid that acts as a transcription factor</t>
+  </si>
+  <si>
+    <t>Major acute phase protein</t>
+  </si>
+  <si>
+    <t>Serum amyloid A-1 protein</t>
+  </si>
+  <si>
+    <t>Acyl-CoA desaturase 1</t>
+  </si>
+  <si>
+    <t>Acute phase</t>
+  </si>
+  <si>
+    <t>Plays an important role in lipid biosynthesis</t>
+  </si>
+  <si>
+    <t>Insulin resistance. Adipokine that modulates insulin action.</t>
+  </si>
+  <si>
+    <t>NAD-dependent protein deacetylase sirtuin-1</t>
+  </si>
+  <si>
+    <t>Biological rhytms and apoptosis</t>
+  </si>
+  <si>
+    <t>Involved in longevity and ageing associated cancer</t>
+  </si>
+  <si>
+    <t>NAD-dependent protein deacetylase sirtuin-3</t>
+  </si>
+  <si>
+    <t>Important for regulating tissue-specific ATP levels</t>
+  </si>
+  <si>
+    <t>Aerobic respiration</t>
+  </si>
+  <si>
+    <t>Solute carrier family 2, facilitated glucose transporter member 2</t>
+  </si>
+  <si>
+    <t>Facilitative hexose transporter that mediates the transport of glucose and fructose</t>
+  </si>
+  <si>
+    <t>Carbohydrate transport</t>
+  </si>
+  <si>
+    <t>Suppressor of cytokine signaling 2</t>
+  </si>
+  <si>
+    <t>Cytokine signaling, IGF signaling. Part of a classical negative feedback system that regulates cytokine signal transduction.</t>
+  </si>
+  <si>
+    <t>Growth regulation</t>
+  </si>
+  <si>
+    <t>Superoxide dismutase</t>
+  </si>
+  <si>
+    <t>Oxygen homeostasis</t>
+  </si>
+  <si>
+    <t>Sterol regulatory element-binding protein 1</t>
+  </si>
+  <si>
+    <t>Key transcription factor that regulates expression of genes involved in cholesterol biosynthesis and lipid homeostasis</t>
+  </si>
+  <si>
+    <t>Transforming growth factor beta-1 proprotein</t>
+  </si>
+  <si>
+    <t>Multifunctional protein that regulates the growth and differentiation of various cell types.</t>
+  </si>
+  <si>
+    <t>Cell growth and differentiation</t>
+  </si>
+  <si>
+    <t>Negative regulation of catalytic process</t>
+  </si>
+  <si>
+    <t>Toll-Like-Receptor 4</t>
+  </si>
+  <si>
+    <t>Mediates the innate immune response to bacterial lipoproteins and other microbial cell wall components.</t>
+  </si>
+  <si>
+    <t>Mediates the innate immune response to bacterial lipopolysaccharide</t>
+  </si>
+  <si>
+    <t>Tumor necrosis factor</t>
+  </si>
+  <si>
+    <t> It is mainly secreted by macrophages and can induce cell death and is a potent pyrogen</t>
+  </si>
+  <si>
+    <t>Inflammatory response</t>
+  </si>
+  <si>
+    <t>Uncouples oxidative phosphorylation from ATP synthesis. As a result, energy is dissipated in the form of heat</t>
+  </si>
+  <si>
+    <t>Mitochondrial uncoupling protein 2</t>
+  </si>
+  <si>
+    <t>Adaptive thermogenesis</t>
+  </si>
+  <si>
+    <t>Peroxisome proliferator-activated receptors signaling pathway</t>
+  </si>
+  <si>
+    <t>Peroxisome proliferator-activated receptors (PPARs) are nuclear hormone receptors that are activated by fatty acids and their derivatives. PPARalpha plays a role in the clearance of circulating or cellular lipids via the regulation of gene expression involved in lipid metabolism in liver and skeletal muscle. PPARbeta/delta is involved in lipid oxidation and cell proliferation. PPARgamma promotes adipocyte differentiation</t>
+  </si>
+  <si>
+    <t>Intracellular signaling pathway important in regulating the cell cycle. It is directly related to cellular quiescence, proliferation, cancer, and longevity. PI3K activation phosphorylates and activates AKT, localizing it in the plasma membrane. AKT can have a number of downstream effects.</t>
+  </si>
+  <si>
+    <t>Mitogen‑activated protein kinase (MAPK) cascades are key signalling pathways that regulate a wide variety of cellular processes, including proliferation, differentiation, apoptosis and stress responses.</t>
+  </si>
+  <si>
+    <t>Mitogen‑activated protein kinase signaling pathway</t>
+  </si>
+  <si>
+    <t>Wnt signaling pathway</t>
+  </si>
+  <si>
+    <t>The Wnt signaling pathway is an ancient and evolutionarily conserved pathway that regulates crucial aspects of cell fate determination, cell migration, cell polarity, neural patterning and organogenesis during embryonic development.</t>
+  </si>
+  <si>
+    <t>Vascular endothelial growth factor pathway</t>
+  </si>
+  <si>
+    <t>VEGF is the most prominent among the angiogenic cytokines and is believed to play a central role in the process of neovascularization, both in cancer as well as other inflammatory diseases.</t>
+  </si>
+  <si>
+    <t>Apoptosis is a form of programmed cell death that occurs in multicellular organisms. Biochemical events lead to characteristic cell changes and death. These changes include blebbing, cell shrinkage, nuclear fragmentation, chromatin condensation, DNA fragmentation and mRNA decay.</t>
+  </si>
+  <si>
+    <t>Apoptosis pathway</t>
+  </si>
+  <si>
+    <t>The TNF signaling pathway plays an important role in various physiological and pathological processes, including cell proliferation, differentiation, apoptosis, and modulation of immune responses and induction of inflammation.</t>
+  </si>
+  <si>
+    <t> Tumour-necrosis factor signaling pathway</t>
+  </si>
+  <si>
+    <t>Toll-like receptors (TLRs) recognize distinct pathogen-associated molecular patterns and play a critical role in innate immune responses</t>
+  </si>
+  <si>
+    <t>Toll-like receptor pathways</t>
   </si>
 </sst>
 </file>
@@ -1652,7 +1916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
@@ -1676,7 +1940,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1690,19 +1954,19 @@
         <v>62</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>3</v>
@@ -1720,7 +1984,7 @@
         <v>43</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>5</v>
@@ -1731,13 +1995,13 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -1764,7 +2028,7 @@
         <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N3" t="s">
         <v>7</v>
@@ -1778,13 +2042,13 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -1811,7 +2075,7 @@
         <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N4" t="s">
         <v>7</v>
@@ -1822,16 +2086,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
         <v>120</v>
-      </c>
-      <c r="C5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" t="s">
-        <v>122</v>
       </c>
       <c r="F5">
         <v>2019</v>
@@ -1843,7 +2107,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
@@ -1860,16 +2124,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
         <v>119</v>
       </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>121</v>
-      </c>
       <c r="E6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F6">
         <v>2019</v>
@@ -1881,7 +2145,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J6" t="s">
         <v>24</v>
@@ -1898,25 +2162,25 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" t="s">
         <v>102</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E7" t="s">
-        <v>104</v>
       </c>
       <c r="F7">
         <v>2019</v>
       </c>
       <c r="G7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H7" s="8">
         <v>7</v>
@@ -1942,25 +2206,25 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F8">
         <v>2019</v>
       </c>
       <c r="G8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H8" s="8">
         <v>9</v>
@@ -1969,7 +2233,7 @@
         <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K8" t="s">
         <v>11</v>
@@ -1992,10 +2256,10 @@
         <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E9" t="s">
         <v>65</v>
@@ -2013,7 +2277,7 @@
         <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K9" t="s">
         <v>11</v>
@@ -2022,13 +2286,13 @@
         <v>32</v>
       </c>
       <c r="M9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N9" t="s">
         <v>7</v>
       </c>
       <c r="O9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2037,24 +2301,24 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="F12">
         <v>2014</v>
@@ -2069,7 +2333,7 @@
         <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K12" t="s">
         <v>11</v>
@@ -2078,36 +2342,36 @@
         <v>32</v>
       </c>
       <c r="M12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N12" t="s">
         <v>27</v>
       </c>
       <c r="O12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" t="s">
         <v>132</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
         <v>133</v>
-      </c>
-      <c r="C13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" t="s">
-        <v>135</v>
       </c>
       <c r="F13">
         <v>2013</v>
       </c>
       <c r="G13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H13" s="8">
         <v>6</v>
@@ -2116,7 +2380,7 @@
         <v>14</v>
       </c>
       <c r="J13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K13" t="s">
         <v>11</v>
@@ -2125,13 +2389,13 @@
         <v>32</v>
       </c>
       <c r="M13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N13" t="s">
         <v>27</v>
       </c>
       <c r="O13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2139,13 +2403,13 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E14" t="s">
         <v>35</v>
@@ -2154,16 +2418,16 @@
         <v>2014</v>
       </c>
       <c r="G14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H14" s="8">
         <v>6</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J14" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K14" t="s">
         <v>11</v>
@@ -2178,12 +2442,12 @@
         <v>27</v>
       </c>
       <c r="O14" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="I16" s="18"/>
     </row>
@@ -2195,10 +2459,10 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D17" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E17" t="s">
         <v>38</v>
@@ -2210,7 +2474,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>14</v>
@@ -2222,45 +2486,45 @@
         <v>33</v>
       </c>
       <c r="M17" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="N17" t="s">
         <v>27</v>
       </c>
       <c r="O17" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" t="s">
         <v>174</v>
       </c>
-      <c r="B18" t="s">
-        <v>175</v>
-      </c>
-      <c r="C18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" t="s">
-        <v>176</v>
-      </c>
       <c r="E18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F18">
         <v>2015</v>
       </c>
       <c r="G18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H18" s="8">
         <v>3</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K18" t="s">
         <v>26</v>
@@ -2269,13 +2533,13 @@
         <v>32</v>
       </c>
       <c r="M18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="N18" t="s">
         <v>27</v>
       </c>
       <c r="O18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2286,10 +2550,10 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -2316,36 +2580,36 @@
         <v>32</v>
       </c>
       <c r="M19" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="N19" t="s">
         <v>7</v>
       </c>
       <c r="O19" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E20" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F20">
         <v>2012</v>
       </c>
       <c r="G20" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H20" s="8">
         <v>2</v>
@@ -2354,60 +2618,60 @@
         <v>13</v>
       </c>
       <c r="J20" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="K20" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="L20" t="s">
         <v>32</v>
       </c>
       <c r="M20" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="N20" t="s">
         <v>27</v>
       </c>
       <c r="O20" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" t="s">
+        <v>279</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" t="s">
         <v>159</v>
-      </c>
-      <c r="B23" t="s">
-        <v>290</v>
-      </c>
-      <c r="C23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E23" t="s">
-        <v>161</v>
       </c>
       <c r="F23">
         <v>2017</v>
       </c>
       <c r="G23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K23" t="s">
         <v>11</v>
@@ -2416,42 +2680,42 @@
         <v>32</v>
       </c>
       <c r="M23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="O23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>240</v>
+      </c>
+      <c r="E24" t="s">
         <v>96</v>
-      </c>
-      <c r="B24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" t="s">
-        <v>248</v>
-      </c>
-      <c r="E24" t="s">
-        <v>98</v>
       </c>
       <c r="F24">
         <v>2015</v>
       </c>
       <c r="G24" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K24" t="s">
         <v>11</v>
@@ -2468,25 +2732,25 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" t="s">
         <v>125</v>
-      </c>
-      <c r="B25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" t="s">
-        <v>127</v>
       </c>
       <c r="F25">
         <v>2014</v>
       </c>
       <c r="G25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H25" s="8">
         <v>2</v>
@@ -2495,7 +2759,7 @@
         <v>14</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K25" t="s">
         <v>11</v>
@@ -2504,7 +2768,7 @@
         <v>32</v>
       </c>
       <c r="M25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N25" t="s">
         <v>27</v>
@@ -2512,7 +2776,7 @@
     </row>
     <row r="27" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="I27" s="18"/>
     </row>
@@ -2521,31 +2785,31 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E28" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="F28">
         <v>2013</v>
       </c>
       <c r="G28" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J28" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="K28" t="s">
         <v>11</v>
@@ -2554,7 +2818,7 @@
         <v>32</v>
       </c>
       <c r="M28" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="N28" t="s">
         <v>27</v>
@@ -2568,16 +2832,16 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D29" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="E29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F29">
         <v>2014</v>
@@ -2586,13 +2850,13 @@
         <v>15</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K29" t="s">
         <v>26</v>
@@ -2601,13 +2865,13 @@
         <v>33</v>
       </c>
       <c r="M29" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="N29" t="s">
         <v>27</v>
       </c>
       <c r="O29" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -2615,13 +2879,13 @@
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E30" t="s">
         <v>45</v>
@@ -2630,7 +2894,7 @@
         <v>2018</v>
       </c>
       <c r="G30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H30" s="8">
         <v>3</v>
@@ -2648,36 +2912,36 @@
         <v>32</v>
       </c>
       <c r="M30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N30" t="s">
         <v>27</v>
       </c>
       <c r="O30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B31" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="C31" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="D31" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="E31" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="F31">
         <v>2017</v>
       </c>
       <c r="G31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H31" s="8">
         <v>6</v>
@@ -2686,7 +2950,7 @@
         <v>14</v>
       </c>
       <c r="J31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K31" t="s">
         <v>11</v>
@@ -2695,13 +2959,13 @@
         <v>32</v>
       </c>
       <c r="M31" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="N31" t="s">
         <v>27</v>
       </c>
       <c r="O31" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2712,10 +2976,10 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
@@ -2727,7 +2991,7 @@
         <v>15</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>14</v>
@@ -2742,7 +3006,7 @@
         <v>33</v>
       </c>
       <c r="M32" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="O32" t="s">
         <v>47</v>
@@ -2753,7 +3017,7 @@
     </row>
     <row r="34" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
@@ -2766,10 +3030,10 @@
         <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E35" t="s">
         <v>0</v>
@@ -2804,34 +3068,34 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F36">
         <v>2019</v>
       </c>
       <c r="G36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H36" s="8">
         <v>3</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K36" t="s">
         <v>11</v>
@@ -2840,36 +3104,36 @@
         <v>50</v>
       </c>
       <c r="M36" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="N36" t="s">
         <v>27</v>
       </c>
       <c r="O36" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F37">
         <v>2017</v>
       </c>
       <c r="G37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H37" s="8">
         <v>3</v>
@@ -2878,16 +3142,16 @@
         <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K37" t="s">
         <v>11</v>
       </c>
       <c r="L37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O37" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -2895,13 +3159,13 @@
     </row>
     <row r="39" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="I39" s="18"/>
     </row>
@@ -2940,7 +3204,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E43" s="13">
         <v>6</v>
@@ -2951,7 +3215,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E44" s="13">
         <v>99</v>
@@ -2963,7 +3227,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="E45" s="21">
         <f>SUM(E40:E44)</f>
@@ -2981,18 +3245,18 @@
     </row>
     <row r="47" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="I47" s="18"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D49">
         <v>5.2</v>
@@ -3000,7 +3264,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D50">
         <v>7.41</v>
@@ -3008,7 +3272,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D51">
         <v>5.1820000000000004</v>
@@ -3026,844 +3290,963 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.85546875" style="25" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>246</v>
+        <v>379</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="26" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="D4" s="26" t="s">
+        <v>376</v>
+      </c>
       <c r="E4" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F5" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="D6" s="26" t="s">
+        <v>378</v>
+      </c>
       <c r="E6" s="26"/>
-      <c r="F6" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>324</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="26" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="26" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="28" t="s">
+        <v>383</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>94</v>
-      </c>
       <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="26" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>390</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="26" t="s">
+      <c r="D10" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F10" s="27" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="26" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>95</v>
-      </c>
       <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="26" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>394</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="26" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27" t="s">
-        <v>286</v>
-      </c>
-      <c r="H13" s="28" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="26" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>60</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="26" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="28" t="s">
+        <v>399</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>358</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>403</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>371</v>
+        <v>350</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>372</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="26" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>406</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="26" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>409</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G19" s="27"/>
-      <c r="H19" s="26" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="26" t="s">
+        <v>411</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>327</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D20" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27" t="s">
-        <v>395</v>
-      </c>
-      <c r="H21" s="26" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>416</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>379</v>
+        <v>357</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>378</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="26" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>418</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B23" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28" t="s">
+        <v>420</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="G23" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>390</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="26" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="28" t="s">
+        <v>423</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>424</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>427</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>426</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="26" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="28" t="s">
+        <v>428</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>429</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>61</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>431</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>430</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="26" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="28" t="s">
+        <v>432</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>433</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="G30" s="27"/>
-      <c r="H30" s="26" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>437</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>434</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27" t="s">
-        <v>303</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>438</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="H32" s="26" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>439</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>441</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>442</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27" t="s">
+      <c r="B34" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="H33" s="26" t="s">
+      <c r="C34" s="28"/>
+      <c r="D34" s="28" t="s">
+        <v>443</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>444</v>
+      </c>
+      <c r="G34" s="26" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="26" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="D35" s="28"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="26" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D35" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>447</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="D36" s="28"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="H36" s="26" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>451</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G37" s="27" t="s">
-        <v>356</v>
-      </c>
-      <c r="H37" s="26" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D37" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>453</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="26" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>454</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>455</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
       <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G39" s="27"/>
-      <c r="H39" s="26" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D39" s="26" t="s">
+        <v>456</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>458</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>457</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C40" s="28"/>
       <c r="D40" s="28" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="F40" s="26"/>
-      <c r="G40" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="H40" s="28" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C41" s="28"/>
       <c r="D41" s="28" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="F41" s="26"/>
-      <c r="G41" s="29" t="s">
-        <v>282</v>
-      </c>
-      <c r="H41" s="28" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="G41" s="28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>381</v>
+        <v>359</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="26" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D42" s="28" t="s">
+        <v>460</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>462</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G43" s="27"/>
-      <c r="H43" s="26" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D43" s="26" t="s">
+        <v>463</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>357</v>
-      </c>
-      <c r="H44" s="26" t="s">
-        <v>363</v>
+      <c r="D44" s="26" t="s">
+        <v>467</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>468</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>466</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1">
+  <autoFilter ref="A1:G1">
     <sortState ref="A2:H44">
       <sortCondition ref="A1"/>
     </sortState>
@@ -3888,16 +4271,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3938,7 +4321,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E5" s="13">
         <v>6</v>
@@ -3949,7 +4332,7 @@
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="B6" s="24"/>
       <c r="E6" s="13">
@@ -3961,7 +4344,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -3982,108 +4365,143 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="D2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>471</v>
+      </c>
+      <c r="D3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4" t="s">
+        <v>473</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="D4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>475</v>
+      </c>
+      <c r="D5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>391</v>
-      </c>
-      <c r="B3" t="s">
-        <v>331</v>
-      </c>
-      <c r="C3" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>329</v>
-      </c>
-      <c r="B4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>332</v>
-      </c>
-      <c r="C5" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>333</v>
-      </c>
-      <c r="C6" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>476</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>477</v>
+      </c>
+      <c r="D6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>335</v>
-      </c>
-      <c r="C7" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="B7" t="s">
+        <v>479</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="D7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>337</v>
-      </c>
-      <c r="C8" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="B8" t="s">
+        <v>481</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>480</v>
+      </c>
+      <c r="D8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>341</v>
-      </c>
-      <c r="C9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>342</v>
-      </c>
-      <c r="B10" t="s">
-        <v>343</v>
-      </c>
-      <c r="C10" t="s">
-        <v>380</v>
+        <v>325</v>
+      </c>
+      <c r="B9" t="s">
+        <v>483</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>482</v>
+      </c>
+      <c r="D9" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>